<commit_message>
correction for sugar in solution
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/data/www/sites/lemoncello/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91B87C0-5ED2-FE4B-B6A9-206CFD477AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98B351F-AADC-C246-9EF9-66DF8793D9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28540" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{1110B225-827B-644C-9DDD-9A5C36A43FED}"/>
+    <workbookView xWindow="-27780" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{1110B225-827B-644C-9DDD-9A5C36A43FED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
+        <f>B11*(B15+$B$4)</f>
         <v>2.7194298574643656</v>
       </c>
       <c r="C19" t="s">

</xml_diff>